<commit_message>
Adding full text search.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/transaction-isolation/isolation-comparison.xlsx
+++ b/hotrod/docs/research/transaction-isolation/isolation-comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,54 +20,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>DB2</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>Read Uncommitted</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>TXs overlap :(</t>
-  </si>
-  <si>
-    <t>Read Committed</t>
-  </si>
-  <si>
-    <t>Repeatable Read</t>
-  </si>
-  <si>
-    <t>First TX fails, Second TX completes</t>
-  </si>
-  <si>
-    <t>First TX completes, Second  TX fails</t>
-  </si>
-  <si>
-    <t>Serializable</t>
-  </si>
-  <si>
-    <t>Cursor Stability</t>
-  </si>
-  <si>
-    <t>Read Stability</t>
-  </si>
-  <si>
-    <t>Snapshot</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Uncommitted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXs overlap *1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXs overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Committed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXs overlap *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeatable Read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First TX fails, Second TX completes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First TX completes, Second  TX fails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read Stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serializable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*1 Called “Uncommitted Read” in DB2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2 Called “Cursor Stability” in DB2.</t>
   </si>
 </sst>
 </file>
@@ -75,13 +84,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,6 +113,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -286,20 +297,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="2" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="2" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -327,110 +339,108 @@
         <v>7</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="5"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>